<commit_message>
Updated project 3 data to 145 data points
</commit_message>
<xml_diff>
--- a/Project_3/Data/year1_gpa.xlsx
+++ b/Project_3/Data/year1_gpa.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="261">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="274">
   <x:si>
     <x:t xml:space="preserve">ID</x:t>
   </x:si>
@@ -809,6 +809,45 @@
   </x:si>
   <x:si>
     <x:t xml:space="preserve">4.56</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">250</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">3.90</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">308</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">4.55</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">4.33</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">333</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">3.65</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">3.43</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">223</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">0.3</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">2.56</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">3.77</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">267</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -905,8 +944,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:AJ132" insertRow="1" totalsRowShown="0">
-  <x:autoFilter ref="A1:AJ132"/>
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:AJ146" insertRow="1" totalsRowShown="0">
+  <x:autoFilter ref="A1:AJ146"/>
   <x:tableColumns count="36">
     <x:tableColumn id="1" uniqueName="1" name="ID" dataDxfId="0"/>
     <x:tableColumn id="2" uniqueName="2" name="Start time" dataDxfId="3"/>
@@ -15248,11 +15287,1495 @@
         <x:v>45</x:v>
       </x:c>
     </x:row>
+    <x:row r="133" hidden="0">
+      <x:c r="A133">
+        <x:v>133</x:v>
+      </x:c>
+      <x:c r="B133" s="2">
+        <x:v>45217.5436805556</x:v>
+      </x:c>
+      <x:c r="C133" s="2">
+        <x:v>45217.5464814815</x:v>
+      </x:c>
+      <x:c r="D133" s="10" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="E133" s="10" t="s"/>
+      <x:c r="F133" s="2"/>
+      <x:c r="G133" s="7" t="s">
+        <x:v>261</x:v>
+      </x:c>
+      <x:c r="H133" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="I133" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="J133" s="10" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="K133" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="L133" s="10" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="M133" s="7" t="s">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="N133" s="10" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="O133" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="P133" s="10" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="Q133">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="R133">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="S133">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="T133">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="U133" s="7" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="V133" s="7" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="W133" s="7" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="X133" s="7" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="Y133" s="7" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="Z133" s="7" t="s">
+        <x:v>105</x:v>
+      </x:c>
+      <x:c r="AA133" s="10" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="AB133" s="10" t="s">
+        <x:v>81</x:v>
+      </x:c>
+      <x:c r="AC133" s="7" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="AD133" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="AE133" s="10" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="AF133" s="10" t="s">
+        <x:v>94</x:v>
+      </x:c>
+      <x:c r="AG133">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="AH133" s="10" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="AI133" s="7" t="s">
+        <x:v>221</x:v>
+      </x:c>
+      <x:c r="AJ133" s="7" t="s">
+        <x:v>45</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="134" hidden="0">
+      <x:c r="A134">
+        <x:v>134</x:v>
+      </x:c>
+      <x:c r="B134" s="2">
+        <x:v>45217.8488888889</x:v>
+      </x:c>
+      <x:c r="C134" s="2">
+        <x:v>45217.8502893519</x:v>
+      </x:c>
+      <x:c r="D134" s="10" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="E134" s="10" t="s"/>
+      <x:c r="F134" s="2"/>
+      <x:c r="G134" s="7" t="s">
+        <x:v>192</x:v>
+      </x:c>
+      <x:c r="H134" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="I134" s="10" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="J134" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="K134" s="10" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="L134" s="10" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="M134" s="7" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="N134" s="10" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="O134" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="P134" s="10" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="Q134">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="R134">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="S134">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="T134">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="U134" s="7" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="V134" s="7" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="W134" s="7" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="X134" s="7" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="Y134" s="7" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="Z134" s="7" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="AA134" s="10" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="AB134" s="10" t="s">
+        <x:v>66</x:v>
+      </x:c>
+      <x:c r="AC134" s="7" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="AD134" s="10" t="s">
+        <x:v>82</x:v>
+      </x:c>
+      <x:c r="AE134" s="10" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="AF134" s="10" t="s">
+        <x:v>98</x:v>
+      </x:c>
+      <x:c r="AG134">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="AH134" s="10" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="AI134" s="7" t="s">
+        <x:v>262</x:v>
+      </x:c>
+      <x:c r="AJ134" s="7" t="s">
+        <x:v>45</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="135" hidden="0">
+      <x:c r="A135">
+        <x:v>135</x:v>
+      </x:c>
+      <x:c r="B135" s="2">
+        <x:v>45224.8482291667</x:v>
+      </x:c>
+      <x:c r="C135" s="2">
+        <x:v>45224.8536342593</x:v>
+      </x:c>
+      <x:c r="D135" s="10" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="E135" s="10" t="s"/>
+      <x:c r="F135" s="2"/>
+      <x:c r="G135" s="7" t="s">
+        <x:v>263</x:v>
+      </x:c>
+      <x:c r="H135" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="I135" s="10" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="J135" s="10" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="K135" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="L135" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="M135" s="7" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="N135" s="10" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="O135" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="P135" s="10" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="Q135">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="R135">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="S135">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="T135">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="U135" s="7" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="V135" s="7" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="W135" s="7" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="X135" s="7" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="Y135" s="7" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="Z135" s="7" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="AA135" s="10" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="AB135" s="10" t="s">
+        <x:v>81</x:v>
+      </x:c>
+      <x:c r="AC135" s="7" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="AD135" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="AE135" s="10" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="AF135" s="10" t="s">
+        <x:v>117</x:v>
+      </x:c>
+      <x:c r="AG135">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="AH135" s="10" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="AI135" s="7" t="s">
+        <x:v>264</x:v>
+      </x:c>
+      <x:c r="AJ135" s="7" t="s">
+        <x:v>45</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="136" hidden="0">
+      <x:c r="A136">
+        <x:v>136</x:v>
+      </x:c>
+      <x:c r="B136" s="2">
+        <x:v>45225.5069791667</x:v>
+      </x:c>
+      <x:c r="C136" s="2">
+        <x:v>45225.5097337963</x:v>
+      </x:c>
+      <x:c r="D136" s="10" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="E136" s="10" t="s"/>
+      <x:c r="F136" s="2"/>
+      <x:c r="G136" s="7" t="s">
+        <x:v>121</x:v>
+      </x:c>
+      <x:c r="H136" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="I136" s="10" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="J136" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="K136" s="10" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="L136" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="M136" s="7" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="N136" s="10" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="O136" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="P136" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="Q136">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="R136">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="S136">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="T136">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="U136" s="7" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="V136" s="7" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="W136" s="7" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="X136" s="7" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="Y136" s="7" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="Z136" s="7" t="s">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="AA136" s="10" t="s">
+        <x:v>151</x:v>
+      </x:c>
+      <x:c r="AB136" s="10" t="s">
+        <x:v>66</x:v>
+      </x:c>
+      <x:c r="AC136" s="7" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="AD136" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="AE136" s="10" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="AF136" s="10" t="s">
+        <x:v>98</x:v>
+      </x:c>
+      <x:c r="AG136">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="AH136" s="10" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="AI136" s="7" t="s">
+        <x:v>265</x:v>
+      </x:c>
+      <x:c r="AJ136" s="7" t="s">
+        <x:v>45</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="137" hidden="0">
+      <x:c r="A137">
+        <x:v>137</x:v>
+      </x:c>
+      <x:c r="B137" s="2">
+        <x:v>45225.5129976852</x:v>
+      </x:c>
+      <x:c r="C137" s="2">
+        <x:v>45225.5146296296</x:v>
+      </x:c>
+      <x:c r="D137" s="10" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="E137" s="10" t="s"/>
+      <x:c r="F137" s="2"/>
+      <x:c r="G137" s="7" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="H137" s="10" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="I137" s="10" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="J137" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="K137" s="10" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="L137" s="10" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="M137" s="7" t="s">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="N137" s="10" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="O137" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="P137" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="Q137">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="R137">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="S137">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="T137">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="U137" s="7" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="V137" s="7" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="W137" s="7" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="X137" s="7" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="Y137" s="7" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="Z137" s="7" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="AA137" s="10" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="AB137" s="10" t="s">
+        <x:v>66</x:v>
+      </x:c>
+      <x:c r="AC137" s="7" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="AD137" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="AE137" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="AF137" s="10" t="s">
+        <x:v>94</x:v>
+      </x:c>
+      <x:c r="AG137">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="AH137" s="10" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="AI137" s="7" t="s">
+        <x:v>115</x:v>
+      </x:c>
+      <x:c r="AJ137" s="7" t="s">
+        <x:v>45</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="138" hidden="0">
+      <x:c r="A138">
+        <x:v>138</x:v>
+      </x:c>
+      <x:c r="B138" s="2">
+        <x:v>45225.5129513889</x:v>
+      </x:c>
+      <x:c r="C138" s="2">
+        <x:v>45225.5170138889</x:v>
+      </x:c>
+      <x:c r="D138" s="10" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="E138" s="10" t="s"/>
+      <x:c r="F138" s="2"/>
+      <x:c r="G138" s="7" t="s">
+        <x:v>266</x:v>
+      </x:c>
+      <x:c r="H138" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="I138" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="J138" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="K138" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="L138" s="10" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="M138" s="7" t="s">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="N138" s="10" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="O138" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="P138" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="Q138">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="R138">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="S138">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="T138">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="U138" s="7" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="V138" s="7" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="W138" s="7" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="X138" s="7" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="Y138" s="7" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="Z138" s="7" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="AA138" s="10" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="AB138" s="10" t="s">
+        <x:v>66</x:v>
+      </x:c>
+      <x:c r="AC138" s="7" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="AD138" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="AE138" s="10" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="AF138" s="10" t="s">
+        <x:v>114</x:v>
+      </x:c>
+      <x:c r="AG138">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="AH138" s="10" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="AI138" s="7" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="AJ138" s="7" t="s">
+        <x:v>45</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="139" hidden="0">
+      <x:c r="A139">
+        <x:v>139</x:v>
+      </x:c>
+      <x:c r="B139" s="2">
+        <x:v>45225.5150694444</x:v>
+      </x:c>
+      <x:c r="C139" s="2">
+        <x:v>45225.5176273148</x:v>
+      </x:c>
+      <x:c r="D139" s="10" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="E139" s="10" t="s"/>
+      <x:c r="F139" s="2"/>
+      <x:c r="G139" s="7" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="H139" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="I139" s="10" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="J139" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="K139" s="10" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="L139" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="M139" s="7" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="N139" s="10" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="O139" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="P139" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="Q139">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="R139">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="S139">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="T139">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="U139" s="7" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="V139" s="7" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="W139" s="7" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="X139" s="7" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="Y139" s="7" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="Z139" s="7" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="AA139" s="10" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="AB139" s="10" t="s">
+        <x:v>81</x:v>
+      </x:c>
+      <x:c r="AC139" s="7" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="AD139" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="AE139" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="AF139" s="10" t="s">
+        <x:v>127</x:v>
+      </x:c>
+      <x:c r="AG139">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="AH139" s="10" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="AI139" s="7" t="s">
+        <x:v>267</x:v>
+      </x:c>
+      <x:c r="AJ139" s="7" t="s">
+        <x:v>45</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="140" hidden="0">
+      <x:c r="A140">
+        <x:v>140</x:v>
+      </x:c>
+      <x:c r="B140" s="2">
+        <x:v>45225.5157175926</x:v>
+      </x:c>
+      <x:c r="C140" s="2">
+        <x:v>45225.5185763889</x:v>
+      </x:c>
+      <x:c r="D140" s="10" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="E140" s="10" t="s"/>
+      <x:c r="F140" s="2"/>
+      <x:c r="G140" s="7" t="s">
+        <x:v>232</x:v>
+      </x:c>
+      <x:c r="H140" s="10" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="I140" s="10" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="J140" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="K140" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="L140" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="M140" s="7" t="s">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="N140" s="10" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="O140" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="P140" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="Q140">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="R140">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="S140">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="T140">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="U140" s="7" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="V140" s="7" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="W140" s="7" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="X140" s="7" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="Y140" s="7" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="Z140" s="7" t="s">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="AA140" s="10" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="AB140" s="10" t="s">
+        <x:v>66</x:v>
+      </x:c>
+      <x:c r="AC140" s="7" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="AD140" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="AE140" s="10" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="AF140" s="10" t="s">
+        <x:v>114</x:v>
+      </x:c>
+      <x:c r="AG140">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="AH140" s="10" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="AI140" s="7" t="s">
+        <x:v>268</x:v>
+      </x:c>
+      <x:c r="AJ140" s="7" t="s">
+        <x:v>45</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="141" hidden="0">
+      <x:c r="A141">
+        <x:v>141</x:v>
+      </x:c>
+      <x:c r="B141" s="2">
+        <x:v>45225.5431481481</x:v>
+      </x:c>
+      <x:c r="C141" s="2">
+        <x:v>45225.5452546296</x:v>
+      </x:c>
+      <x:c r="D141" s="10" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="E141" s="10" t="s"/>
+      <x:c r="F141" s="2"/>
+      <x:c r="G141" s="7" t="s">
+        <x:v>269</x:v>
+      </x:c>
+      <x:c r="H141" s="10" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="I141" s="10" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="J141" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="K141" s="10" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="L141" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="M141" s="7" t="s">
+        <x:v>86</x:v>
+      </x:c>
+      <x:c r="N141" s="10" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="O141" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="P141" s="10" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="Q141">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="R141">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="S141">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="T141">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="U141" s="7" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="V141" s="7" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="W141" s="7" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="X141" s="7" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="Y141" s="7" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="Z141" s="7" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="AA141" s="10" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="AB141" s="10" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="AC141" s="7" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="AD141" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="AE141" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="AF141" s="10" t="s">
+        <x:v>98</x:v>
+      </x:c>
+      <x:c r="AG141">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="AH141" s="10" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="AI141" s="7" t="s">
+        <x:v>190</x:v>
+      </x:c>
+      <x:c r="AJ141" s="7" t="s">
+        <x:v>45</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="142" hidden="0">
+      <x:c r="A142">
+        <x:v>142</x:v>
+      </x:c>
+      <x:c r="B142" s="2">
+        <x:v>45225.5701388889</x:v>
+      </x:c>
+      <x:c r="C142" s="2">
+        <x:v>45225.5763657407</x:v>
+      </x:c>
+      <x:c r="D142" s="10" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="E142" s="10" t="s"/>
+      <x:c r="F142" s="2"/>
+      <x:c r="G142" s="7" t="s">
+        <x:v>234</x:v>
+      </x:c>
+      <x:c r="H142" s="10" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="I142" s="10" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="J142" s="10" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="K142" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="L142" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="M142" s="7" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="N142" s="10" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="O142" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="P142" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="Q142">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="R142">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="S142">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="T142">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="U142" s="7" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="V142" s="7" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="W142" s="7" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="X142" s="7" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="Y142" s="7" t="s">
+        <x:v>270</x:v>
+      </x:c>
+      <x:c r="Z142" s="7" t="s">
+        <x:v>256</x:v>
+      </x:c>
+      <x:c r="AA142" s="10" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="AB142" s="10" t="s">
+        <x:v>81</x:v>
+      </x:c>
+      <x:c r="AC142" s="7" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="AD142" s="10" t="s">
+        <x:v>82</x:v>
+      </x:c>
+      <x:c r="AE142" s="10" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="AF142" s="10" t="s">
+        <x:v>117</x:v>
+      </x:c>
+      <x:c r="AG142">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="AH142" s="10" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="AI142" s="7" t="s">
+        <x:v>271</x:v>
+      </x:c>
+      <x:c r="AJ142" s="7" t="s">
+        <x:v>45</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="143" hidden="0">
+      <x:c r="A143">
+        <x:v>143</x:v>
+      </x:c>
+      <x:c r="B143" s="2">
+        <x:v>45225.5851273148</x:v>
+      </x:c>
+      <x:c r="C143" s="2">
+        <x:v>45225.5877777778</x:v>
+      </x:c>
+      <x:c r="D143" s="10" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="E143" s="10" t="s"/>
+      <x:c r="F143" s="2"/>
+      <x:c r="G143" s="7" t="s">
+        <x:v>80</x:v>
+      </x:c>
+      <x:c r="H143" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="I143" s="10" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="J143" s="10" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="K143" s="10" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="L143" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="M143" s="7" t="s">
+        <x:v>78</x:v>
+      </x:c>
+      <x:c r="N143" s="10" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="O143" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="P143" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="Q143">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="R143">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="S143">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="T143">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="U143" s="7" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="V143" s="7" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="W143" s="7" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="X143" s="7" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="Y143" s="7" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="Z143" s="7" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="AA143" s="10" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="AB143" s="10" t="s">
+        <x:v>81</x:v>
+      </x:c>
+      <x:c r="AC143" s="7" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="AD143" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="AE143" s="10" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="AF143" s="10" t="s">
+        <x:v>94</x:v>
+      </x:c>
+      <x:c r="AG143">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="AH143" s="10" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="AI143" s="7" t="s">
+        <x:v>115</x:v>
+      </x:c>
+      <x:c r="AJ143" s="7" t="s">
+        <x:v>45</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="144" hidden="0">
+      <x:c r="A144">
+        <x:v>144</x:v>
+      </x:c>
+      <x:c r="B144" s="2">
+        <x:v>45225.5913425926</x:v>
+      </x:c>
+      <x:c r="C144" s="2">
+        <x:v>45225.593275463</x:v>
+      </x:c>
+      <x:c r="D144" s="10" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="E144" s="10" t="s"/>
+      <x:c r="F144" s="2"/>
+      <x:c r="G144" s="7" t="s">
+        <x:v>143</x:v>
+      </x:c>
+      <x:c r="H144" s="10" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="I144" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="J144" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="K144" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="L144" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="M144" s="7" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="N144" s="10" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="O144" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="P144" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="Q144">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="R144">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="S144">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="T144">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="U144" s="7" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="V144" s="7" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="W144" s="7" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="X144" s="7" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="Y144" s="7" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="Z144" s="7" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="AA144" s="10" t="s">
+        <x:v>151</x:v>
+      </x:c>
+      <x:c r="AB144" s="10" t="s">
+        <x:v>81</x:v>
+      </x:c>
+      <x:c r="AC144" s="7" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="AD144" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="AE144" s="10" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="AF144" s="10" t="s">
+        <x:v>114</x:v>
+      </x:c>
+      <x:c r="AG144">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="AH144" s="10" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="AI144" s="7" t="s">
+        <x:v>272</x:v>
+      </x:c>
+      <x:c r="AJ144" s="7" t="s">
+        <x:v>45</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="145" hidden="0">
+      <x:c r="A145">
+        <x:v>145</x:v>
+      </x:c>
+      <x:c r="B145" s="2">
+        <x:v>45225.5924421296</x:v>
+      </x:c>
+      <x:c r="C145" s="2">
+        <x:v>45225.5944444444</x:v>
+      </x:c>
+      <x:c r="D145" s="10" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="E145" s="10" t="s"/>
+      <x:c r="F145" s="2"/>
+      <x:c r="G145" s="7" t="s">
+        <x:v>273</x:v>
+      </x:c>
+      <x:c r="H145" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="I145" s="10" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="J145" s="10" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="K145" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="L145" s="10" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="M145" s="7" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="N145" s="10" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="O145" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="P145" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="Q145">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="R145">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="S145">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="T145">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="U145" s="7" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="V145" s="7" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="W145" s="7" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="X145" s="7" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="Y145" s="7" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="Z145" s="7" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="AA145" s="10" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="AB145" s="10" t="s">
+        <x:v>81</x:v>
+      </x:c>
+      <x:c r="AC145" s="7" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="AD145" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="AE145" s="10" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="AF145" s="10" t="s">
+        <x:v>114</x:v>
+      </x:c>
+      <x:c r="AG145">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="AH145" s="10" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="AI145" s="7" t="s">
+        <x:v>264</x:v>
+      </x:c>
+      <x:c r="AJ145" s="7" t="s">
+        <x:v>45</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="146" hidden="0">
+      <x:c r="A146">
+        <x:v>146</x:v>
+      </x:c>
+      <x:c r="B146" s="2">
+        <x:v>45225.7096180556</x:v>
+      </x:c>
+      <x:c r="C146" s="2">
+        <x:v>45225.7119444444</x:v>
+      </x:c>
+      <x:c r="D146" s="10" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="E146" s="10" t="s"/>
+      <x:c r="F146" s="2"/>
+      <x:c r="G146" s="7" t="s">
+        <x:v>156</x:v>
+      </x:c>
+      <x:c r="H146" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="I146" s="10" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="J146" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="K146" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="L146" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="M146" s="7" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="N146" s="10" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="O146" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="P146" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="Q146">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="R146">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="S146">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="T146">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="U146" s="7" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="V146" s="7" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="W146" s="7" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="X146" s="7" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="Y146" s="7" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="Z146" s="7" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="AA146" s="10" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="AB146" s="10" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AC146" s="7" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="AD146" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="AE146" s="10" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="AF146" s="10" t="s">
+        <x:v>114</x:v>
+      </x:c>
+      <x:c r="AG146">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="AH146" s="10" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="AI146" s="7" t="s">
+        <x:v>161</x:v>
+      </x:c>
+      <x:c r="AJ146" s="7" t="s">
+        <x:v>45</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <x:pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <x:tableParts count="1">
-    <x:tablePart r:id="R8d7c67d7d07d4393"/>
+    <x:tablePart r:id="R56e14adb6fe74cdf"/>
   </x:tableParts>
 </x:worksheet>
 </file>
</xml_diff>